<commit_message>
Deploying to gh-pages from  @ 2259ed271aafbe375bc8a6c016181d5e137bd14c 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/10.3.1.xlsx
+++ b/en/downloads/data-excel/10.3.1.xlsx
@@ -44,12 +44,6 @@
     <t>Items</t>
   </si>
   <si>
-    <t xml:space="preserve"> Көп көрсөткүчтүү кластердик изилдөөнүн маалыматтары боюнча, 2018-ж.</t>
-  </si>
-  <si>
-    <t>По данным кластерного обследования по многим показателям, 2018г.</t>
-  </si>
-  <si>
     <t>Местность</t>
   </si>
   <si>
@@ -134,9 +128,6 @@
     <t>Богатейший</t>
   </si>
   <si>
-    <t xml:space="preserve"> 10.3.1 Доля женщин, сообщивших об испытанных ими лично в последние 12 месяцев проявлениях дискриминации или преследованиях на основании дискриминации, которая запрещена международным правом</t>
-  </si>
-  <si>
     <t>10.3.1 Proportion of women reporting having personally felt discriminated against or harassed in the previous 12 months on the basis of a ground of discrimination prohibited under international human rights law</t>
   </si>
   <si>
@@ -278,9 +269,6 @@
     <t xml:space="preserve"> 10.3.1 Акыркы 12 ай ичинде эл аралык укук менен тыюу салынган дискриминациянын негизинде жеке өзүнүн башынан өткөн дискриминация көрүнүштөрү же куугунтуктар жөнүндө алар өздөрү маалымдаган аялдардын үлүшү</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Акыркы 12 ай ичинде өзүнө карата дискриминацияны же бардык белгилери боюнча кысым көрсөтүүлөрдү сезген 15-49 жаштагы аялдардын пайыздык үлүшү</t>
   </si>
   <si>
@@ -290,9 +278,6 @@
     <t>Жетиштүү жашоо индексинин квинтили</t>
   </si>
   <si>
-    <t>According to the cluster survey for many indicators, 2018.</t>
-  </si>
-  <si>
     <t>Функционалдык кыйынчылыктары (жашы: 18-49 жаш)</t>
   </si>
   <si>
@@ -363,6 +348,21 @@
   </si>
   <si>
     <t>By education</t>
+  </si>
+  <si>
+    <t>10.3.1 Доля женщин, сообщивших о том, что в последние 12 месяцев они лично подвергались дискриминации или преследованиям на основаниях, дискриминация по которым запрещена в соответствии с международными стандартами в области прав человека</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Көп көрсөткүчтүү кластердик изилдөөнүн маалыматтары боюнча, 2018-ж., 2023-ж.</t>
+  </si>
+  <si>
+    <t>По данным кластерного обследования по многим показателям, 2018г., 2023г.</t>
+  </si>
+  <si>
+    <t>According to the cluster survey for many indicators, 2018, 2023</t>
+  </si>
+  <si>
+    <t>(18,7)</t>
   </si>
 </sst>
 </file>
@@ -926,15 +926,15 @@
     <col min="3" max="3" width="41.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>36</v>
+        <v>108</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -966,556 +966,661 @@
       <c r="D4" s="3">
         <v>2018</v>
       </c>
+      <c r="E4" s="3">
+        <v>2023</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D5" s="34">
         <v>7.7</v>
       </c>
-      <c r="E5" t="s">
-        <v>84</v>
+      <c r="E5" s="34">
+        <v>6.2</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
     </row>
     <row r="7" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D7" s="13">
         <v>7.9</v>
       </c>
+      <c r="E7" s="13">
+        <v>7.4</v>
+      </c>
     </row>
     <row r="8" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D8" s="13">
         <v>7.6</v>
       </c>
+      <c r="E8" s="13">
+        <v>5.6</v>
+      </c>
     </row>
     <row r="9" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
     </row>
     <row r="10" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D10" s="13">
         <v>0.4</v>
       </c>
+      <c r="E10" s="13">
+        <v>4.3</v>
+      </c>
     </row>
     <row r="11" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D11" s="13">
         <v>7.3</v>
       </c>
+      <c r="E11" s="13">
+        <v>7.1</v>
+      </c>
     </row>
     <row r="12" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D12" s="13">
         <v>1.7</v>
       </c>
+      <c r="E12" s="13">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="13" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D13" s="13">
         <v>2.8</v>
       </c>
+      <c r="E13" s="13">
+        <v>2.9</v>
+      </c>
     </row>
     <row r="14" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D14" s="13">
         <v>6.5</v>
       </c>
+      <c r="E14" s="13">
+        <v>3.4</v>
+      </c>
     </row>
     <row r="15" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D15" s="19">
         <v>5</v>
       </c>
+      <c r="E15" s="19">
+        <v>1.9</v>
+      </c>
     </row>
     <row r="16" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D16" s="13">
         <v>16.600000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E16" s="13">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D17" s="13">
         <v>8.6999999999999993</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="13">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D18" s="19">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="19">
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D19" s="13"/>
-    </row>
-    <row r="20" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="13"/>
+    </row>
+    <row r="20" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D20" s="13">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="13">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D21" s="13">
         <v>5.7</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="13">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D22" s="13">
         <v>8.3000000000000007</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E22" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D23" s="13">
         <v>9.1</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E23" s="13">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D24" s="13">
         <v>7.1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E24" s="13">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D25" s="13">
         <v>8.8000000000000007</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="13">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D26" s="13">
         <v>8.6999999999999993</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E26" s="13">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D27" s="13">
         <v>6.4</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E27" s="13">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D28" s="19">
         <v>7</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E28" s="19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C29" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+    </row>
+    <row r="30" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="D29" s="13"/>
-    </row>
-    <row r="30" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C30" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D31" s="19">
         <v>14</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E31" s="19">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="29" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C32" s="24" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D32" s="19">
         <v>5.9</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E32" s="19">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="29" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D33" s="19">
         <v>6.9</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E33" s="19">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D34" s="19">
         <v>8.1999999999999993</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" s="14" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="E34" s="19">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="14" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A35" s="35" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D35" s="19"/>
-    </row>
-    <row r="36" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E35" s="19"/>
+    </row>
+    <row r="36" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D36" s="19">
         <v>20.7</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E36" s="19">
+        <v>32.299999999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D37" s="19">
         <v>7.6</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E37" s="19">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D38" s="19"/>
-    </row>
-    <row r="39" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E38" s="19"/>
+    </row>
+    <row r="39" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="32" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D39" s="19">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E39" s="19">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="32" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D40" s="19">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E40" s="19">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="32" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C41" s="24" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D41" s="19">
         <v>9.6999999999999993</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E41" s="19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="32" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D42" s="19">
         <v>7.1</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" s="14" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E42" s="19">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="14" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D43" s="21">
         <v>8.8000000000000007</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E43" s="21">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="36" t="s">
-        <v>6</v>
+        <v>109</v>
       </c>
       <c r="B44" s="36" t="s">
-        <v>7</v>
+        <v>110</v>
       </c>
       <c r="C44" s="36" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ 6860cd36a4b5e2909e862fc5ac1c51dcabfb5495 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/10.3.1.xlsx
+++ b/en/downloads/data-excel/10.3.1.xlsx
@@ -359,10 +359,10 @@
     <t>По данным кластерного обследования по многим показателям, 2018г., 2023г.</t>
   </si>
   <si>
-    <t>According to the cluster survey for many indicators, 2018, 2023</t>
-  </si>
-  <si>
     <t>(18,7)</t>
+  </si>
+  <si>
+    <t>According to Multiple Indicator Cluster Survey, 2018, 2023.</t>
   </si>
 </sst>
 </file>
@@ -917,7 +917,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1393,7 +1395,7 @@
         <v>35</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1617,7 +1619,7 @@
         <v>110</v>
       </c>
       <c r="C44" s="36" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>